<commit_message>
add Spanish bert - BETO and update status
</commit_message>
<xml_diff>
--- a/status.xlsx
+++ b/status.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gal\Documents\Gong project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>dir_name</t>
   </si>
@@ -282,13 +282,24 @@
   </si>
   <si>
     <t>size of val (ES)</t>
+  </si>
+  <si>
+    <t>translation_transformer_Helsinki_eng_to_es/BETO</t>
+  </si>
+  <si>
+    <t>translated EN ds to ES using Helsinki (20000).
+Embedding using Spanish BERT.
+Train with the translated ds and test with es.</t>
+  </si>
+  <si>
+    <t>finiteautomata/beto-sentiment-analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +332,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -340,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -413,9 +431,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="9"/>
-      </left>
+      <left/>
       <right/>
       <top style="medium">
         <color theme="9"/>
@@ -424,32 +440,120 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
       <right/>
       <top style="medium">
         <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="9"/>
-      </right>
-      <top style="medium">
-        <color theme="9"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="9"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -462,7 +566,9 @@
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -471,43 +577,8 @@
         <color theme="9"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF7030A0"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF7030A0"/>
-      </top>
       <bottom style="medium">
-        <color rgb="FF7030A0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF7030A0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF7030A0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF7030A0"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF7030A0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF7030A0"/>
+        <color theme="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,7 +588,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -532,19 +603,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -827,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I8"/>
+  <dimension ref="A3:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,10 +997,10 @@
       <c r="E5" s="1">
         <v>2500</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <v>0.88600000000000001</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>0.55400000000000005</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -929,40 +1009,40 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="19">
+        <v>6600</v>
+      </c>
+      <c r="E6" s="19">
+        <v>2500</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="13">
-        <v>20000</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6600</v>
-      </c>
-      <c r="E6" s="11">
-        <v>2500</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0.877</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0.82</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>20000</v>
       </c>
       <c r="D7" s="1">
@@ -972,42 +1052,75 @@
         <v>2500</v>
       </c>
       <c r="F7" s="1">
+        <v>0.877</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="25">
+        <v>20000</v>
+      </c>
+      <c r="D8" s="26">
+        <v>6600</v>
+      </c>
+      <c r="E8" s="26">
+        <v>2500</v>
+      </c>
+      <c r="F8" s="26">
         <v>0.92600000000000005</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G8" s="26">
         <v>0.85399999999999998</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I8" s="27"/>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="18" t="s">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C9" s="13">
         <v>223549</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D9" s="13">
         <v>73772</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E9" s="13">
         <v>2500</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F9" s="13">
         <v>0.95799999999999996</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G9" s="13">
         <v>0.87</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add train results to predict notebook and update status
</commit_message>
<xml_diff>
--- a/status.xlsx
+++ b/status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>dir_name</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>finiteautomata/beto-sentiment-analysis</t>
+  </si>
+  <si>
+    <t>ROC AUC train</t>
   </si>
 </sst>
 </file>
@@ -340,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +360,12 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -588,7 +597,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,6 +634,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -907,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I17"/>
+  <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,12 +933,14 @@
     <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -945,16 +960,19 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -974,14 +992,17 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="G4" s="5">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="H4" s="5">
         <v>0.86299999999999999</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1001,14 +1022,17 @@
         <v>0.88600000000000001</v>
       </c>
       <c r="G5" s="10">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="H5" s="10">
         <v>0.55400000000000005</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
@@ -1027,15 +1051,18 @@
       <c r="F6" s="20">
         <v>0.92800000000000005</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="29">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="H6" s="20">
         <v>0.85099999999999998</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -1051,18 +1078,21 @@
       <c r="E7" s="1">
         <v>2500</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="28">
         <v>0.877</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="28">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="H7" s="28">
         <v>0.82</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="23" t="s">
         <v>14</v>
       </c>
@@ -1082,14 +1112,17 @@
         <v>0.92600000000000005</v>
       </c>
       <c r="G8" s="26">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="H8" s="26">
         <v>0.85399999999999998</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="I8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
@@ -1109,14 +1142,17 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="G9" s="13">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="H9" s="13">
         <v>0.87</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>